<commit_message>
buat alert untuk pendaftaran dan rapihin segala macamnya
</commit_message>
<xml_diff>
--- a/admin/Data_Pendaftar.xlsx
+++ b/admin/Data_Pendaftar.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
   <si>
     <t>DATA DIRI PENDAFTAR MTS ASSAADAH 2025</t>
   </si>
@@ -149,7 +149,7 @@
     <t>Bandung</t>
   </si>
   <si>
-    <t>2024-11-30</t>
+    <t>2003-05-31</t>
   </si>
   <si>
     <t>L</t>
@@ -158,13 +158,13 @@
     <t>islam</t>
   </si>
   <si>
-    <t>bodjoeng</t>
+    <t>Jl tambun rengas rt 03/rw 07 Cakung timur Jakarta timur</t>
   </si>
   <si>
     <t>agus@gmail.com</t>
   </si>
   <si>
-    <t>088888888</t>
+    <t>087888868291</t>
   </si>
   <si>
     <t>main hoha</t>
@@ -203,16 +203,16 @@
     <t>pns</t>
   </si>
   <si>
-    <t>New</t>
-  </si>
-  <si>
-    <t>amin</t>
-  </si>
-  <si>
-    <t>bekasi</t>
-  </si>
-  <si>
-    <t>2001-01-30</t>
+    <t>Checked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sabrina </t>
+  </si>
+  <si>
+    <t>solo</t>
+  </si>
+  <si>
+    <t>2000-06-30</t>
   </si>
   <si>
     <t>P</t>
@@ -221,106 +221,37 @@
     <t>budha</t>
   </si>
   <si>
-    <t>Jl tambun rengas rt 03/rw 07 Cakung timur Jakarta timur</t>
-  </si>
-  <si>
-    <t>amin@gmail.com</t>
-  </si>
-  <si>
-    <t>081905212457</t>
-  </si>
-  <si>
-    <t>da</t>
-  </si>
-  <si>
-    <t>ad</t>
+    <t>bekasi tarjay</t>
+  </si>
+  <si>
+    <t>sabre@gmail.com</t>
+  </si>
+  <si>
+    <t>ngoding</t>
+  </si>
+  <si>
+    <t>selebgram</t>
   </si>
   <si>
     <t>Imunisasi Lengkap</t>
   </si>
   <si>
-    <t>tr</t>
+    <t>man 21</t>
+  </si>
+  <si>
+    <t>dodi</t>
+  </si>
+  <si>
+    <t>pedagang</t>
   </si>
   <si>
     <t>3000.000 - 5000.000</t>
   </si>
   <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>Checked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">damas hadi </t>
-  </si>
-  <si>
-    <t>Jakarta</t>
-  </si>
-  <si>
-    <t>kristen</t>
-  </si>
-  <si>
-    <t>jakut</t>
-  </si>
-  <si>
-    <t>damas@gmail.com</t>
-  </si>
-  <si>
-    <t>main bola</t>
-  </si>
-  <si>
-    <t>bm playfield</t>
-  </si>
-  <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <t>1000.000 - 2000.000</t>
-  </si>
-  <si>
-    <t>Fahad Ahmad Boenjamin</t>
-  </si>
-  <si>
-    <t>JAKARTA</t>
-  </si>
-  <si>
-    <t>2025-02-19</t>
-  </si>
-  <si>
-    <t>Jl Perkici EB 1 No.10</t>
-  </si>
-  <si>
-    <t>elfahad@gmail.com</t>
-  </si>
-  <si>
-    <t>0812937152738</t>
-  </si>
-  <si>
-    <t>SMA</t>
-  </si>
-  <si>
-    <t>2000.000 - 3000.000</t>
-  </si>
-  <si>
-    <t>Fatur Rahman</t>
-  </si>
-  <si>
-    <t>2002-02-12</t>
-  </si>
-  <si>
-    <t>fatur988@gmail.com</t>
-  </si>
-  <si>
-    <t>programer</t>
-  </si>
-  <si>
-    <t>mi assaadah</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>neneng</t>
+    <t>maya</t>
+  </si>
+  <si>
+    <t>hrd</t>
   </si>
 </sst>
 </file>
@@ -682,7 +613,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AO7"/>
+  <dimension ref="A1:AO4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="AO2" sqref="AO2"/>
@@ -691,21 +622,21 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="25.851" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="10.569" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="6.998" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="65.984" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="22.28" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="12.854" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="10.569" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="11.711" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="15.282" bestFit="true" customWidth="true" style="0"/>
@@ -718,7 +649,7 @@
     <col min="26" max="26" width="10.569" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="10.569" bestFit="true" customWidth="true" style="0"/>
     <col min="28" max="28" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="12.854" bestFit="true" customWidth="true" style="0"/>
+    <col min="29" max="29" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="30" max="30" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="31" max="31" width="25.851" bestFit="true" customWidth="true" style="0"/>
     <col min="32" max="32" width="11.711" bestFit="true" customWidth="true" style="0"/>
@@ -868,7 +799,7 @@
         <v>47</v>
       </c>
       <c r="B3">
-        <v>2020112233</v>
+        <v>18191010</v>
       </c>
       <c r="C3" t="s">
         <v>42</v>
@@ -969,10 +900,10 @@
     </row>
     <row r="4" spans="1:41">
       <c r="A4">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B4">
-        <v>2412515</v>
+        <v>18191010</v>
       </c>
       <c r="C4" t="s">
         <v>63</v>
@@ -995,41 +926,41 @@
       <c r="I4" t="s">
         <v>69</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4">
+        <v>123456789</v>
+      </c>
+      <c r="K4">
+        <v>1231241</v>
+      </c>
+      <c r="L4">
+        <v>12321451</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
         <v>70</v>
       </c>
-      <c r="K4">
-        <v>132312</v>
-      </c>
-      <c r="L4">
-        <v>234234</v>
-      </c>
-      <c r="M4">
-        <v>2</v>
-      </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>71</v>
-      </c>
-      <c r="P4" t="s">
-        <v>72</v>
       </c>
       <c r="Q4" t="s">
         <v>52</v>
       </c>
       <c r="R4" t="s">
+        <v>72</v>
+      </c>
+      <c r="S4" t="s">
         <v>73</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>74</v>
       </c>
-      <c r="T4" t="s">
-        <v>72</v>
-      </c>
       <c r="U4">
-        <v>0</v>
+        <v>1224123</v>
       </c>
       <c r="V4" t="s">
         <v>60</v>
@@ -1038,28 +969,28 @@
         <v>2147483647</v>
       </c>
       <c r="X4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="Y4" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z4">
-        <v>13</v>
+        <v>76</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>77</v>
       </c>
       <c r="AA4">
-        <v>123</v>
+        <v>31241241</v>
       </c>
       <c r="AB4" t="s">
         <v>60</v>
       </c>
       <c r="AC4">
-        <v>2147483647</v>
+        <v>78903234</v>
       </c>
       <c r="AD4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE4" t="s">
         <v>76</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>75</v>
       </c>
       <c r="AG4">
         <v>0</v>
@@ -1067,328 +998,7 @@
       <c r="AL4">
         <v>0</v>
       </c>
-      <c r="AM4">
-        <v>213</v>
-      </c>
-      <c r="AN4">
-        <v>123</v>
-      </c>
       <c r="AO4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:41">
-      <c r="A5">
-        <v>49</v>
-      </c>
-      <c r="B5">
-        <v>123456</v>
-      </c>
-      <c r="C5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J5" t="s">
-        <v>70</v>
-      </c>
-      <c r="K5">
-        <v>1241234132</v>
-      </c>
-      <c r="L5">
-        <v>1212313113</v>
-      </c>
-      <c r="M5">
-        <v>2</v>
-      </c>
-      <c r="N5">
-        <v>2</v>
-      </c>
-      <c r="O5" t="s">
-        <v>83</v>
-      </c>
-      <c r="P5" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>52</v>
-      </c>
-      <c r="R5" t="s">
-        <v>73</v>
-      </c>
-      <c r="S5" t="s">
-        <v>54</v>
-      </c>
-      <c r="T5" t="s">
-        <v>63</v>
-      </c>
-      <c r="U5">
-        <v>1234</v>
-      </c>
-      <c r="V5" t="s">
-        <v>85</v>
-      </c>
-      <c r="W5">
-        <v>2147483647</v>
-      </c>
-      <c r="X5" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA5">
-        <v>12312313</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AC5">
-        <v>884838482</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG5">
-        <v>0</v>
-      </c>
-      <c r="AL5">
-        <v>0</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:41">
-      <c r="A6">
-        <v>50</v>
-      </c>
-      <c r="B6">
-        <v>1237816237</v>
-      </c>
-      <c r="C6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" t="s">
-        <v>89</v>
-      </c>
-      <c r="F6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" t="s">
-        <v>91</v>
-      </c>
-      <c r="J6" t="s">
-        <v>92</v>
-      </c>
-      <c r="K6">
-        <v>132312</v>
-      </c>
-      <c r="L6">
-        <v>123312</v>
-      </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
-      <c r="N6">
-        <v>2</v>
-      </c>
-      <c r="O6" t="s">
-        <v>71</v>
-      </c>
-      <c r="P6" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>52</v>
-      </c>
-      <c r="S6" t="s">
-        <v>72</v>
-      </c>
-      <c r="T6" t="s">
-        <v>72</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6" t="s">
-        <v>93</v>
-      </c>
-      <c r="W6">
-        <v>123</v>
-      </c>
-      <c r="X6" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z6">
-        <v>13</v>
-      </c>
-      <c r="AA6">
-        <v>123</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC6">
-        <v>123</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>76</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>94</v>
-      </c>
-      <c r="AG6">
-        <v>0</v>
-      </c>
-      <c r="AL6">
-        <v>0</v>
-      </c>
-      <c r="AM6">
-        <v>213</v>
-      </c>
-      <c r="AN6">
-        <v>123</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:41">
-      <c r="A7">
-        <v>46</v>
-      </c>
-      <c r="B7">
-        <v>18191010</v>
-      </c>
-      <c r="C7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H7" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J7" t="s">
-        <v>70</v>
-      </c>
-      <c r="K7">
-        <v>1241234132</v>
-      </c>
-      <c r="L7">
-        <v>1212313113</v>
-      </c>
-      <c r="M7">
-        <v>2</v>
-      </c>
-      <c r="N7">
-        <v>2</v>
-      </c>
-      <c r="O7" t="s">
-        <v>83</v>
-      </c>
-      <c r="P7" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>52</v>
-      </c>
-      <c r="R7" t="s">
-        <v>53</v>
-      </c>
-      <c r="S7" t="s">
-        <v>99</v>
-      </c>
-      <c r="T7" t="s">
-        <v>63</v>
-      </c>
-      <c r="U7">
-        <v>12345678</v>
-      </c>
-      <c r="V7" t="s">
-        <v>100</v>
-      </c>
-      <c r="W7">
-        <v>2147483647</v>
-      </c>
-      <c r="X7" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA7">
-        <v>12312313</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AC7">
-        <v>884838482</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG7">
-        <v>0</v>
-      </c>
-      <c r="AL7">
-        <v>0</v>
-      </c>
-      <c r="AO7" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>